<commit_message>
Changed API Results to include ALL cell parse
Changed API form a choice between values and "all" (value, format,
styles, border, alignment, size, formulas, etc), and simply just changed
the single API to always get all of the parsable data. The divergence
from the original forked library is so great now both in code base, code
purpose and API entry and API results, that I've decided to just move
this project to its own project rather than continue as a fork that will
never be merged in. I am thankful to the original creator, and hopefully
this isn't seen as bad practice...

Updated tests. Now pull virtually everything you can garner from the xml
storage of excel sheets. Unfortunately, the color codes and shading
codes they store in xml arent exactly easily transferable to CSS. FIXME
TODO.

Additionally, multi sheet workbooks is not yet supported. Next commit.
</commit_message>
<xml_diff>
--- a/test/spreadsheets/excel_mac_2008-formula.xlsx
+++ b/test/spreadsheets/excel_mac_2008-formula.xlsx
@@ -22,14 +22,18 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>bob</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -59,8 +63,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +398,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -411,12 +416,12 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>